<commit_message>
update entrevitas y subentrevistas
</commit_message>
<xml_diff>
--- a/php/aco_uploads/Listado de Alumnos Sede Colonial.xlsx
+++ b/php/aco_uploads/Listado de Alumnos Sede Colonial.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9080" uniqueCount="3981">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9078" uniqueCount="3981">
   <si>
     <t>77600913</t>
   </si>
@@ -15665,9 +15665,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1258"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15797,12 +15797,8 @@
       <c r="H3" s="18" t="s">
         <v>1476</v>
       </c>
-      <c r="I3" s="18" t="s">
-        <v>1410</v>
-      </c>
-      <c r="J3" s="18" t="s">
-        <v>1152</v>
-      </c>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
       <c r="K3" s="18" t="s">
         <v>3538</v>
       </c>
@@ -62941,6 +62937,15 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="AK2:AL2"/>
+    <mergeCell ref="AM2:AN2"/>
+    <mergeCell ref="AO2:AP2"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="AA2:AB2"/>
+    <mergeCell ref="AC2:AD2"/>
+    <mergeCell ref="AE2:AF2"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="AI2:AJ2"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="W2:X2"/>
@@ -62954,15 +62959,6 @@
     <mergeCell ref="Q2:R2"/>
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="U2:V2"/>
-    <mergeCell ref="AK2:AL2"/>
-    <mergeCell ref="AM2:AN2"/>
-    <mergeCell ref="AO2:AP2"/>
-    <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="AA2:AB2"/>
-    <mergeCell ref="AC2:AD2"/>
-    <mergeCell ref="AE2:AF2"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="AI2:AJ2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
agregar modulos de consultas y reportes
</commit_message>
<xml_diff>
--- a/php/aco_uploads/Listado de Alumnos Sede Colonial.xlsx
+++ b/php/aco_uploads/Listado de Alumnos Sede Colonial.xlsx
@@ -15665,9 +15665,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A1233" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1248" sqref="D1248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -62937,15 +62937,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="AK2:AL2"/>
-    <mergeCell ref="AM2:AN2"/>
-    <mergeCell ref="AO2:AP2"/>
-    <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="AA2:AB2"/>
-    <mergeCell ref="AC2:AD2"/>
-    <mergeCell ref="AE2:AF2"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="AI2:AJ2"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="W2:X2"/>
@@ -62959,6 +62950,15 @@
     <mergeCell ref="Q2:R2"/>
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="U2:V2"/>
+    <mergeCell ref="AK2:AL2"/>
+    <mergeCell ref="AM2:AN2"/>
+    <mergeCell ref="AO2:AP2"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="AA2:AB2"/>
+    <mergeCell ref="AC2:AD2"/>
+    <mergeCell ref="AE2:AF2"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="AI2:AJ2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>